<commit_message>
Edited example/config.xlsx to solve error in column selection for type_population_table()
</commit_message>
<xml_diff>
--- a/data/respons_fake.xlsx
+++ b/data/respons_fake.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vrln.sharepoint.com/sites/GGD-ONDZ/PSchijf/Gezondheidsmonitor/Algemeen/Automatisering en R/0. Github/report_excel_to_powerpoint/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8457249E-3027-45DE-AA23-A2B31D5F3410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{8457249E-3027-45DE-AA23-A2B31D5F3410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5CECB950-4592-4931-A667-54415E985FF8}"/>
   <bookViews>
-    <workbookView xWindow="29190" yWindow="390" windowWidth="24945" windowHeight="11385" xr2:uid="{3FBA482A-4E0F-499D-944B-77EBC58D198C}"/>
+    <workbookView xWindow="-4695" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{3FBA482A-4E0F-499D-944B-77EBC58D198C}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -443,15 +443,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5344762C-110F-42FE-83D0-B259DDA26BAE}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.125" customWidth="1"/>
-    <col min="2" max="2" width="16.375" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="1" max="1" width="18.90625" customWidth="1"/>
+    <col min="2" max="2" width="16.36328125" customWidth="1"/>
+    <col min="3" max="3" width="19.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -554,5 +552,359 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Bedrijfsvertrouwelijk (BBN1)</oddFooter>
+  </headerFooter>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C4EA295FB1FB9547A73C9F5819D6E613" ma:contentTypeVersion="22" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="c6ed9d5736a8b6bce7fdd25df6dc73c6">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4e95bed8-6d15-4403-ad70-a53422338dca" xmlns:ns3="10d3344f-2d16-43d9-a145-97142f5cb288" xmlns:ns4="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9b8dd8ae3f6086a1cec4bb961aaa59ad" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
+    <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
+    <xsd:import namespace="4e95bed8-6d15-4403-ad70-a53422338dca"/>
+    <xsd:import namespace="10d3344f-2d16-43d9-a145-97142f5cb288"/>
+    <xsd:import namespace="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns4:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyProperties" minOccurs="0"/>
+                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyUIAction" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns4:TaxKeywordTaxHTField" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="http://schemas.microsoft.com/sharepoint/v3" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="24" nillable="true" ma:displayName="Eigenschappen van het geïntegreerd beleid voor naleving" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="25" nillable="true" ma:displayName="Actie van de gebruikersinterface van het geïntegreerd beleid voor naleving" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="4e95bed8-6d15-4403-ad70-a53422338dca" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="11" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="12" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="13" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="14" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="15" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="19" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="21" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Afbeeldingtags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="6a01bbcf-c6fe-4904-b3d7-d8e248b039cf" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="23" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="26" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="27" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="10d3344f-2d16-43d9-a145-97142f5cb288" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="17" nillable="true" ma:displayName="Gedeeld met" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="18" nillable="true" ma:displayName="Gedeeld met details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="22" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{fa7ae801-cb9e-41d3-a15b-605146dc1d91}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="10d3344f-2d16-43d9-a145-97142f5cb288">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TaxKeywordTaxHTField" ma:index="29" nillable="true" ma:taxonomy="true" ma:internalName="TaxKeywordTaxHTField" ma:taxonomyFieldName="TaxKeyword" ma:displayName="Ondernemingstrefwoorden" ma:fieldId="{23f27201-bee3-471e-b2e7-b64fd8b7ca38}" ma:taxonomyMulti="true" ma:sspId="6a01bbcf-c6fe-4904-b3d7-d8e248b039cf" ma:termSetId="00000000-0000-0000-0000-000000000000" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="true" ma:isKeyword="true">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Inhoudstype"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titel"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxKeywordTaxHTField xmlns="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4e95bed8-6d15-4403-ad70-a53422338dca">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A96D75BE-5D25-4205-A673-244AD00F25DE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="4e95bed8-6d15-4403-ad70-a53422338dca"/>
+    <ds:schemaRef ds:uri="10d3344f-2d16-43d9-a145-97142f5cb288"/>
+    <ds:schemaRef ds:uri="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E419E566-6C31-47FB-8031-B8659AB0364F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="d045ab76-3bb7-45f5-ab41-d7b04aa0dc94"/>
+    <ds:schemaRef ds:uri="4e95bed8-6d15-4403-ad70-a53422338dca"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48DF5B8D-ACF3-4B9E-BCA1-196D554B2A29}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>